<commit_message>
got rid of old matricies
</commit_message>
<xml_diff>
--- a/cod_figures/regressions/regressions_all_in_one.xlsx
+++ b/cod_figures/regressions/regressions_all_in_one.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\provo\Documents\GitHub\popdy\cod_figures\regressions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B0972A82-D280-42A7-A001-0BC11935CFF6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{25288CFE-B74E-4A79-B0E0-BB60736936B3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9450" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="37">
   <si>
     <t>Table 1</t>
   </si>
   <si>
-    <t>Lambda 1 vs. Peak spawning age (mode)</t>
-  </si>
-  <si>
     <t>standard error of the slope</t>
   </si>
   <si>
@@ -103,9 +100,6 @@
     <t>Standard deviation vs k</t>
   </si>
   <si>
-    <t>Table 4</t>
-  </si>
-  <si>
     <t>Damping ratio (lambda2/lambda1) vs CV of spawning biomass distribution</t>
   </si>
   <si>
@@ -116,6 +110,27 @@
   </si>
   <si>
     <t>term</t>
+  </si>
+  <si>
+    <t>Lambda 1 vs. CV about the mode</t>
+  </si>
+  <si>
+    <t>Table 4b</t>
+  </si>
+  <si>
+    <t>Table 4a</t>
+  </si>
+  <si>
+    <t>Mean 1/rho as a function of k</t>
+  </si>
+  <si>
+    <t>Does variation in CV depend on mode or stdev? Ans: mode</t>
+  </si>
+  <si>
+    <t>Stdev</t>
+  </si>
+  <si>
+    <t>Mode</t>
   </si>
 </sst>
 </file>
@@ -258,7 +273,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -436,6 +451,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -599,9 +620,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -957,10 +979,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:F21"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,38 +992,38 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" t="s">
         <v>1</v>
-      </c>
-      <c r="L1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="L2" t="s">
         <v>7</v>
-      </c>
-      <c r="L2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1010,30 +1032,30 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4">
-        <v>0.60429424200000004</v>
+        <v>0.93300300447329199</v>
       </c>
       <c r="D4">
-        <v>6.1069542999999997E-2</v>
+        <v>8.9134986797090796E-2</v>
       </c>
       <c r="E4">
-        <v>9.8951820119999994</v>
+        <v>10.4673040070921</v>
       </c>
       <c r="F4" s="1">
-        <v>5.7399999999999998E-8</v>
+        <v>2.7309542265903498E-8</v>
       </c>
       <c r="G4" t="str">
         <f>IF(F4&lt;=0.001,"***",IF(AND(F4&gt;0.001,F4&lt;=0.01),"**",IF(AND(F4&gt;0.01,F4&lt;=0.05),"*","")))</f>
@@ -1042,127 +1064,127 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5">
-        <v>3.6534324999999999E-2</v>
+        <v>-0.29008117910117398</v>
       </c>
       <c r="D5">
-        <v>1.0055771E-2</v>
+        <v>0.20497423780226201</v>
       </c>
       <c r="E5">
-        <v>3.633170051</v>
+        <v>-1.4152079900939301</v>
       </c>
       <c r="F5">
-        <v>2.4530260000000001E-3</v>
+        <v>0.17743288847543101</v>
       </c>
       <c r="G5" t="str">
-        <f t="shared" ref="G5:G45" si="0">IF(F5&lt;=0.001,"***",IF(AND(F5&gt;0.001,F5&lt;=0.01),"**",IF(AND(F5&gt;0.01,F5&lt;=0.05),"*","")))</f>
-        <v>**</v>
+        <f t="shared" ref="G5:G58" si="0">IF(F5&lt;=0.001,"***",IF(AND(F5&gt;0.001,F5&lt;=0.01),"**",IF(AND(F5&gt;0.01,F5&lt;=0.05),"*","")))</f>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>1.0051076722260699</v>
+      </c>
+      <c r="D6">
+        <v>9.0837541689425705E-2</v>
+      </c>
+      <c r="E6">
+        <v>11.064892923484701</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.2992864372689801E-8</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>***</v>
+      </c>
+      <c r="I6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" t="s">
         <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <v>0.79604875600000002</v>
-      </c>
-      <c r="D6">
-        <v>7.2245707000000006E-2</v>
-      </c>
-      <c r="E6">
-        <v>11.018630610000001</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1.37E-8</v>
-      </c>
-      <c r="G6" t="str">
-        <f t="shared" si="0"/>
-        <v>***</v>
-      </c>
-      <c r="I6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7">
-        <v>2.4516630000000001E-2</v>
+        <v>-0.166862277352606</v>
       </c>
       <c r="D7">
-        <v>1.1896049000000001E-2</v>
+        <v>0.208889421995504</v>
       </c>
       <c r="E7">
-        <v>2.0609052999999999</v>
+        <v>-0.798806735920775</v>
       </c>
       <c r="F7">
-        <v>5.7092437000000003E-2</v>
+        <v>0.43686858276589802</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" t="s">
         <v>17</v>
-      </c>
-      <c r="J7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>1.0407187551474399</v>
+      </c>
+      <c r="D8">
+        <v>9.5857601663927497E-2</v>
+      </c>
+      <c r="E8">
+        <v>10.856924616121301</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1.6764358881614098E-8</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>***</v>
+      </c>
+      <c r="I8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>0.92569727899999998</v>
-      </c>
-      <c r="D8">
-        <v>8.1443584999999999E-2</v>
-      </c>
-      <c r="E8">
-        <v>11.366116529999999</v>
-      </c>
-      <c r="F8" s="1">
-        <v>9.0400000000000002E-9</v>
-      </c>
-      <c r="G8" t="str">
-        <f t="shared" si="0"/>
-        <v>***</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>20</v>
-      </c>
-      <c r="J8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9">
-        <v>1.5181925000000001E-2</v>
+        <v>-6.8499262800923597E-2</v>
       </c>
       <c r="D9">
-        <v>1.341058E-2</v>
+        <v>0.220433519369272</v>
       </c>
       <c r="E9">
-        <v>1.132085577</v>
+        <v>-0.31074794340225997</v>
       </c>
       <c r="F9">
-        <v>0.27537213900000002</v>
+        <v>0.76026856048456504</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
@@ -1171,22 +1193,22 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10">
-        <v>0.99687346399999999</v>
+        <v>1.0568780337685799</v>
       </c>
       <c r="D10">
-        <v>8.6949909000000006E-2</v>
+        <v>0.100046412920825</v>
       </c>
       <c r="E10">
-        <v>11.464916649999999</v>
+        <v>10.5638773336629</v>
       </c>
       <c r="F10" s="1">
-        <v>8.0399999999999995E-9</v>
+        <v>2.4166755128983602E-8</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
@@ -1195,19 +1217,19 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11">
-        <v>9.7436310000000009E-3</v>
+        <v>-1.0634994432931699E-2</v>
       </c>
       <c r="D11">
-        <v>1.4317257E-2</v>
+        <v>0.23006608258078301</v>
       </c>
       <c r="E11">
-        <v>0.68055154600000001</v>
+        <v>-4.6225824830991399E-2</v>
       </c>
       <c r="F11">
-        <v>0.506525004</v>
+        <v>0.96374007721128596</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
@@ -1216,29 +1238,29 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
         <v>23</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
         <v>3</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>4</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>5</v>
-      </c>
-      <c r="F14" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15">
         <v>0.76728353203223998</v>
@@ -1259,7 +1281,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>0.29774058703749201</v>
@@ -1280,29 +1302,29 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
         <v>25</v>
-      </c>
-      <c r="B18" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
         <v>3</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>4</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>5</v>
-      </c>
-      <c r="F19" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20">
         <v>0.110791619689385</v>
@@ -1323,7 +1345,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21">
         <v>7.9538057628636798E-3</v>
@@ -1344,32 +1366,32 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
         <v>3</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>4</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>5</v>
-      </c>
-      <c r="F24" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
         <v>9</v>
-      </c>
-      <c r="B25" t="s">
-        <v>10</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1378,10 +1400,10 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
@@ -1390,10 +1412,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C26">
         <v>0.99513122300000001</v>
@@ -1414,7 +1436,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C27">
         <v>-0.40232742399999999</v>
@@ -1435,10 +1457,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C28">
         <v>1.002068052</v>
@@ -1459,7 +1481,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C29">
         <v>-0.520269329</v>
@@ -1480,10 +1502,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C30">
         <v>1.002088275</v>
@@ -1504,7 +1526,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C31">
         <v>-0.56970507400000003</v>
@@ -1525,10 +1547,10 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C32">
         <v>1.0018786180000001</v>
@@ -1549,7 +1571,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C33">
         <v>-0.59337197600000002</v>
@@ -1570,182 +1592,111 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37">
+        <v>7.9561400392991893E-2</v>
+      </c>
+      <c r="D37">
+        <v>5.8493368142339399E-3</v>
+      </c>
+      <c r="E37">
+        <v>13.601781350560101</v>
+      </c>
+      <c r="F37">
+        <v>5.3617258342222099E-3</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="0"/>
+        <v>**</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38">
+        <v>3.65984279375514E-2</v>
+      </c>
+      <c r="D38">
+        <v>8.42088954063956E-3</v>
+      </c>
+      <c r="E38">
+        <v>4.3461474896358503</v>
+      </c>
+      <c r="F38">
+        <v>4.90763336275922E-2</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="0"/>
+        <v>*</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>29</v>
       </c>
-      <c r="B35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="C42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
         <v>3</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E42" t="s">
         <v>4</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F42" t="s">
         <v>5</v>
       </c>
-      <c r="F36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" t="s">
         <v>9</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
         <v>10</v>
       </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37" t="s">
-        <v>11</v>
-      </c>
-      <c r="F37" t="s">
-        <v>11</v>
-      </c>
-      <c r="G37" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="F43" t="s">
         <v>10</v>
-      </c>
-      <c r="C38">
-        <v>0.34938300500000002</v>
-      </c>
-      <c r="D38">
-        <v>0.134188735</v>
-      </c>
-      <c r="E38">
-        <v>2.6036686680000001</v>
-      </c>
-      <c r="F38">
-        <v>1.9952732000000001E-2</v>
-      </c>
-      <c r="G38" t="str">
-        <f t="shared" si="0"/>
-        <v>*</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39">
-        <v>3.0324169000000002E-2</v>
-      </c>
-      <c r="D39">
-        <v>6.0463253000000002E-2</v>
-      </c>
-      <c r="E39">
-        <v>0.50153056299999998</v>
-      </c>
-      <c r="F39">
-        <v>0.62327825999999997</v>
-      </c>
-      <c r="G39" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>15</v>
-      </c>
-      <c r="B40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40">
-        <v>0.34938300500000002</v>
-      </c>
-      <c r="D40">
-        <v>0.134188735</v>
-      </c>
-      <c r="E40">
-        <v>2.6036686680000001</v>
-      </c>
-      <c r="F40">
-        <v>1.9952732000000001E-2</v>
-      </c>
-      <c r="G40" t="str">
-        <f t="shared" si="0"/>
-        <v>*</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41">
-        <v>3.0324169000000002E-2</v>
-      </c>
-      <c r="D41">
-        <v>6.0463253000000002E-2</v>
-      </c>
-      <c r="E41">
-        <v>0.50153056299999998</v>
-      </c>
-      <c r="F41">
-        <v>0.62327825999999997</v>
-      </c>
-      <c r="G41" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" t="s">
-        <v>10</v>
-      </c>
-      <c r="C42">
-        <v>0.34938300500000002</v>
-      </c>
-      <c r="D42">
-        <v>0.134188735</v>
-      </c>
-      <c r="E42">
-        <v>2.6036686680000001</v>
-      </c>
-      <c r="F42">
-        <v>1.9952732000000001E-2</v>
-      </c>
-      <c r="G42" t="str">
-        <f t="shared" si="0"/>
-        <v>*</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C43">
-        <v>3.0324169000000002E-2</v>
-      </c>
-      <c r="D43">
-        <v>6.0463253000000002E-2</v>
-      </c>
-      <c r="E43">
-        <v>0.50153056299999998</v>
-      </c>
-      <c r="F43">
-        <v>0.62327825999999997</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
@@ -1754,10 +1705,10 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C44">
         <v>0.34938300500000002</v>
@@ -1778,7 +1729,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C45">
         <v>3.0324169000000002E-2</v>
@@ -1795,6 +1746,253 @@
       <c r="G45" t="str">
         <f t="shared" si="0"/>
         <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46">
+        <v>0.34938300500000002</v>
+      </c>
+      <c r="D46">
+        <v>0.134188735</v>
+      </c>
+      <c r="E46">
+        <v>2.6036686680000001</v>
+      </c>
+      <c r="F46">
+        <v>1.9952732000000001E-2</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="0"/>
+        <v>*</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47">
+        <v>3.0324169000000002E-2</v>
+      </c>
+      <c r="D47">
+        <v>6.0463253000000002E-2</v>
+      </c>
+      <c r="E47">
+        <v>0.50153056299999998</v>
+      </c>
+      <c r="F47">
+        <v>0.62327825999999997</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48">
+        <v>0.34938300500000002</v>
+      </c>
+      <c r="D48">
+        <v>0.134188735</v>
+      </c>
+      <c r="E48">
+        <v>2.6036686680000001</v>
+      </c>
+      <c r="F48">
+        <v>1.9952732000000001E-2</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="0"/>
+        <v>*</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49">
+        <v>3.0324169000000002E-2</v>
+      </c>
+      <c r="D49">
+        <v>6.0463253000000002E-2</v>
+      </c>
+      <c r="E49">
+        <v>0.50153056299999998</v>
+      </c>
+      <c r="F49">
+        <v>0.62327825999999997</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50">
+        <v>0.34938300500000002</v>
+      </c>
+      <c r="D50">
+        <v>0.134188735</v>
+      </c>
+      <c r="E50">
+        <v>2.6036686680000001</v>
+      </c>
+      <c r="F50">
+        <v>1.9952732000000001E-2</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="0"/>
+        <v>*</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51">
+        <v>3.0324169000000002E-2</v>
+      </c>
+      <c r="D51">
+        <v>6.0463253000000002E-2</v>
+      </c>
+      <c r="E51">
+        <v>0.50153056299999998</v>
+      </c>
+      <c r="F51">
+        <v>0.62327825999999997</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54" t="s">
+        <v>3</v>
+      </c>
+      <c r="E54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F54" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>35</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55">
+        <v>0.34938300536656702</v>
+      </c>
+      <c r="D55">
+        <v>0.13418873515485399</v>
+      </c>
+      <c r="E55">
+        <v>2.6036686683377699</v>
+      </c>
+      <c r="F55">
+        <v>1.9952732148515399E-2</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="0"/>
+        <v>*</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56">
+        <v>3.0324169123835499E-2</v>
+      </c>
+      <c r="D56">
+        <v>6.0463252589521503E-2</v>
+      </c>
+      <c r="E56">
+        <v>0.50153056319518596</v>
+      </c>
+      <c r="F56">
+        <v>0.62327826008278397</v>
+      </c>
+      <c r="G56" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>36</v>
+      </c>
+      <c r="B57" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57">
+        <v>0.70057125390299002</v>
+      </c>
+      <c r="D57">
+        <v>6.0297161561393899E-2</v>
+      </c>
+      <c r="E57">
+        <v>11.618643991884699</v>
+      </c>
+      <c r="F57" s="1">
+        <v>6.7126916757335603E-9</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" si="0"/>
+        <v>***</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58">
+        <v>-5.0130426419529202E-2</v>
+      </c>
+      <c r="D58">
+        <v>9.9285895866652405E-3</v>
+      </c>
+      <c r="E58">
+        <v>-5.0490984627723696</v>
+      </c>
+      <c r="F58">
+        <v>1.44018136754859E-4</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" si="0"/>
+        <v>***</v>
       </c>
     </row>
   </sheetData>

</xml_diff>